<commit_message>
day 16 part 2 - generate right values from test data but does nt perform operators
</commit_message>
<xml_diff>
--- a/Day16/working.xlsx
+++ b/Day16/working.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tesco-my.sharepoint.com/personal/craig_roberts_tesco_com/Documents/Dev/AdventOfCode/2021/day16/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="315" documentId="8_{DE27C539-B4E9-034B-81D1-60109751F3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{279CF4DD-E764-8B44-9D93-A191DE8E98EF}"/>
+  <xr:revisionPtr revIDLastSave="318" documentId="8_{DE27C539-B4E9-034B-81D1-60109751F3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9793F79-DF39-8542-A0C0-4E7FB85C9887}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" activeTab="3" xr2:uid="{06ABC176-24F0-5840-98D4-2975E874B492}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
   <si>
     <t>100010100000000001001010100000000001101010000000000000101111010001111000</t>
   </si>
@@ -119,7 +119,10 @@
     <t>000001000000000001011010110000110011100010010000</t>
   </si>
   <si>
-    <t>min</t>
+    <t>product</t>
+  </si>
+  <si>
+    <t>lit</t>
   </si>
 </sst>
 </file>
@@ -4971,7 +4974,7 @@
   <dimension ref="A1:DB18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5745,6 +5748,9 @@
       <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:106" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="F4" s="12">
         <f>BIN2DEC(F3)</f>
         <v>1</v>
@@ -6028,7 +6034,7 @@
     </row>
     <row r="9" spans="1:106" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="12">
         <f>BIN2DEC(F8)</f>
@@ -6092,7 +6098,7 @@
     </row>
     <row r="15" spans="1:106" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F15" s="12">
         <f>BIN2DEC(F14)</f>

</xml_diff>